<commit_message>
Exam algorithm and thir gui is done with little fixes in algorithm.
</commit_message>
<xml_diff>
--- a/exam_schedule.xlsx
+++ b/exam_schedule.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -511,12 +511,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -544,12 +544,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -577,12 +577,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -643,12 +643,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -676,12 +676,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -709,12 +709,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -775,12 +775,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -808,12 +808,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -841,12 +841,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -879,7 +879,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -907,12 +907,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -940,12 +940,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -973,12 +973,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1039,12 +1039,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1072,12 +1072,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1105,12 +1105,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1171,12 +1171,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1204,12 +1204,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1237,12 +1237,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1303,12 +1303,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1336,12 +1336,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1402,12 +1402,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1435,12 +1435,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1534,12 +1534,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1600,12 +1600,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1633,12 +1633,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1699,12 +1699,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1732,12 +1732,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">

</xml_diff>